<commit_message>
Updated final results and fixed model
</commit_message>
<xml_diff>
--- a/Social charging model/SCM_export_results_behaviours.xlsx
+++ b/Social charging model/SCM_export_results_behaviours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naudl\Documents\GitHub\social-charging-model\Social charging model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4050C924-E5FB-4E2A-A0DD-65220E7C2CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902B9DF7-F216-4A0A-B8DA-CE39AE26134B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3758AFA0-8E81-488E-A41A-47B84DA45D8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3758AFA0-8E81-488E-A41A-47B84DA45D8A}"/>
   </bookViews>
   <sheets>
     <sheet name="per_week" sheetId="2" r:id="rId1"/>
@@ -778,11 +778,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C276F534-E875-46ED-80D0-6FDBCE465A6B}">
   <dimension ref="A1:DQ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CR7468" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="CD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:DQ7489"/>
+      <selection pane="bottomRight" activeCell="CP2" sqref="CP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>